<commit_message>
Index limit for heldkarp (without interface)
</commit_message>
<xml_diff>
--- a/PerformanceTests/ShortestPathPerformanceTest.xlsx
+++ b/PerformanceTests/ShortestPathPerformanceTest.xlsx
@@ -1,201 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="15990" windowHeight="9000"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Nós</t>
+    <t xml:space="preserve">Nós</t>
   </si>
   <si>
-    <t>A*</t>
+    <t xml:space="preserve">A*</t>
   </si>
   <si>
-    <t>Dijkstra</t>
+    <t xml:space="preserve">Dijkstra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="7">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="14"/>
+      <color rgb="FF595959"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="9"/>
+      <color rgb="FF595959"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,619 +91,187 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
-    <border>
+  <borders count="2">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
-    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
-    <cellStyle name="Title" xfId="40" builtinId="15"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
-    <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <colors>
-    <mruColors>
-      <color rgb="00FFFFFF"/>
-    </mruColors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFBFBFBF"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF5B9BD5"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFD9D9D9"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFED7D31"/>
+      <rgbColor rgb="FF595959"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr vertOverflow="ellipsis" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr algn="ctr" defTabSz="914400">
-              <a:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0">
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="x-none" altLang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:effectLst/>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Tempo(ms)</a:t>
+              <a:t>Tempo (μs)</a:t>
             </a:r>
-            <a:endParaRPr lang="x-none" altLang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="marker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -834,38 +288,43 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="19080">
               <a:noFill/>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="5b9bd5"/>
               </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
+              <a:ln w="19080">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="5b9bd5"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -1024,38 +483,43 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:solidFill>
+              <a:srgbClr val="ed7d31"/>
+            </a:solidFill>
+            <a:ln w="19080">
               <a:noFill/>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="ed7d31"/>
               </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
+              <a:ln w="19080">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:srgbClr val="ed7d31"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -1182,25 +646,28 @@
                 <c:pt idx="15">
                   <c:v>18466</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v/>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="r"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="641602172"/>
-        <c:axId val="617018186"/>
+        <c:axId val="11205415"/>
+        <c:axId val="23548185"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="641602172"/>
+        <c:axId val="11205415"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45000"/>
@@ -1209,61 +676,50 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9360">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:srgbClr val="d9d9d9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9360">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:srgbClr val="bfbfbf"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
-          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
+          <a:bodyPr/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" kern="1200">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="617018186"/>
+        <c:crossAx val="23548185"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="617018186"/>
+        <c:axId val="23548185"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20000"/>
@@ -1273,56 +729,45 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9360">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:srgbClr val="d9d9d9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9360">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:srgbClr val="bfbfbf"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
-          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
+          <a:bodyPr/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" kern="1200">
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="641602172"/>
+        <c:crossAx val="11205415"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1331,662 +776,58 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
-        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
-        <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <a:ln w="9360">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:srgbClr val="d9d9d9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
-    <a:effectLst/>
   </c:spPr>
-  <c:txPr>
-    <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" horzOverflow="overflow" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr lang="en-US" sz="1000" kern="1200">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:latin typeface="+mn-lt"/>
-          <a:ea typeface="+mn-ea"/>
-          <a:cs typeface="+mn-cs"/>
-        </a:defRPr>
-      </a:pPr>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins r="0.7" b="0.75" l="0.7" footer="0.3" header="0.3" t="0.75"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>115570</xdr:colOff>
+      <xdr:colOff>115560</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>111760</xdr:rowOff>
+      <xdr:rowOff>111600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
+      <xdr:colOff>180720</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>197485</xdr:rowOff>
+      <xdr:rowOff>196920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="0" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3163570" y="330835"/>
-        <a:ext cx="6161405" cy="4029075"/>
+        <a:off x="3277800" y="330480"/>
+        <a:ext cx="6389640" cy="4028760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1999,274 +840,23 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="D3DAE3"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="404552"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AW46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="17.25"/>
+  <sheetFormatPr defaultRowHeight="17.25"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.89068825910931"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2323,14 +913,14 @@
       <c r="AV1" s="3"/>
       <c r="AW1" s="3"/>
     </row>
-    <row r="2" spans="1:49">
-      <c r="A2" s="1">
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="1" t="n">
         <v>17</v>
       </c>
       <c r="D2" s="1"/>
@@ -2380,14 +970,14 @@
       <c r="AV2" s="3"/>
       <c r="AW2" s="3"/>
     </row>
-    <row r="3" spans="1:49">
-      <c r="A3" s="1">
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1" t="n">
         <v>144</v>
       </c>
       <c r="D3" s="1"/>
@@ -2437,14 +1027,14 @@
       <c r="AV3" s="3"/>
       <c r="AW3" s="3"/>
     </row>
-    <row r="4" spans="1:49">
-      <c r="A4" s="1">
+    <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
         <v>900</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="n">
         <v>365</v>
       </c>
       <c r="D4" s="1"/>
@@ -2494,14 +1084,14 @@
       <c r="AV4" s="3"/>
       <c r="AW4" s="3"/>
     </row>
-    <row r="5" spans="1:49">
-      <c r="A5" s="1">
+    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
         <v>1600</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="n">
         <v>778</v>
       </c>
       <c r="D5" s="1"/>
@@ -2551,14 +1141,14 @@
       <c r="AV5" s="3"/>
       <c r="AW5" s="3"/>
     </row>
-    <row r="6" spans="1:49">
-      <c r="A6" s="1">
+    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
         <v>2500</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="n">
         <v>186</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="n">
         <v>1391</v>
       </c>
       <c r="D6" s="1"/>
@@ -2608,14 +1198,14 @@
       <c r="AV6" s="3"/>
       <c r="AW6" s="3"/>
     </row>
-    <row r="7" spans="1:49">
-      <c r="A7" s="1">
+    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
         <v>3600</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="1" t="n">
         <v>258</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="n">
         <v>2300</v>
       </c>
       <c r="D7" s="1"/>
@@ -2665,14 +1255,14 @@
       <c r="AV7" s="3"/>
       <c r="AW7" s="3"/>
     </row>
-    <row r="8" spans="1:49">
-      <c r="A8" s="1">
+    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
         <v>4900</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="1" t="n">
         <v>405</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="n">
         <v>3193</v>
       </c>
       <c r="D8" s="1"/>
@@ -2722,14 +1312,14 @@
       <c r="AV8" s="3"/>
       <c r="AW8" s="3"/>
     </row>
-    <row r="9" spans="1:49">
-      <c r="A9" s="1">
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
         <v>6400</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="1" t="n">
         <v>517</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="1" t="n">
         <v>4202</v>
       </c>
       <c r="D9" s="1"/>
@@ -2779,14 +1369,14 @@
       <c r="AV9" s="3"/>
       <c r="AW9" s="3"/>
     </row>
-    <row r="10" spans="1:49">
-      <c r="A10" s="1">
+    <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
         <v>8100</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="n">
         <v>820</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="1" t="n">
         <v>5715</v>
       </c>
       <c r="D10" s="1"/>
@@ -2836,14 +1426,14 @@
       <c r="AV10" s="3"/>
       <c r="AW10" s="3"/>
     </row>
-    <row r="11" spans="1:49">
-      <c r="A11" s="1">
+    <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
         <v>10000</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="1" t="n">
         <v>928</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="n">
         <v>6818</v>
       </c>
       <c r="D11" s="1"/>
@@ -2893,14 +1483,14 @@
       <c r="AV11" s="3"/>
       <c r="AW11" s="3"/>
     </row>
-    <row r="12" spans="1:49">
-      <c r="A12" s="1">
+    <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>12100</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="1" t="n">
         <v>1336</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="1" t="n">
         <v>8001</v>
       </c>
       <c r="D12" s="1"/>
@@ -2950,14 +1540,14 @@
       <c r="AV12" s="3"/>
       <c r="AW12" s="3"/>
     </row>
-    <row r="13" spans="1:49">
-      <c r="A13" s="1">
+    <row r="13" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
         <v>14400</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="1" t="n">
         <v>1488</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="1" t="n">
         <v>10385</v>
       </c>
       <c r="D13" s="1"/>
@@ -3007,14 +1597,14 @@
       <c r="AV13" s="3"/>
       <c r="AW13" s="3"/>
     </row>
-    <row r="14" spans="1:49">
-      <c r="A14" s="1">
+    <row r="14" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
         <v>16900</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="1" t="n">
         <v>2024</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="1" t="n">
         <v>12052</v>
       </c>
       <c r="D14" s="1"/>
@@ -3064,14 +1654,14 @@
       <c r="AV14" s="3"/>
       <c r="AW14" s="3"/>
     </row>
-    <row r="15" spans="1:49">
-      <c r="A15" s="1">
+    <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
         <v>19600</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1" t="n">
         <v>2483</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="1" t="n">
         <v>13993</v>
       </c>
       <c r="D15" s="1"/>
@@ -3121,14 +1711,14 @@
       <c r="AV15" s="3"/>
       <c r="AW15" s="3"/>
     </row>
-    <row r="16" spans="1:49">
-      <c r="A16" s="1">
+    <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
         <v>22500</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1" t="n">
         <v>2453</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="1" t="n">
         <v>16197</v>
       </c>
       <c r="D16" s="1"/>
@@ -3178,14 +1768,14 @@
       <c r="AV16" s="3"/>
       <c r="AW16" s="3"/>
     </row>
-    <row r="17" spans="1:49">
-      <c r="A17" s="1">
+    <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
         <v>25600</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="1" t="n">
         <v>3357</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="1" t="n">
         <v>18466</v>
       </c>
       <c r="D17" s="1"/>
@@ -3235,11 +1825,11 @@
       <c r="AV17" s="3"/>
       <c r="AW17" s="3"/>
     </row>
-    <row r="18" spans="1:49">
-      <c r="A18" s="1">
+    <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
         <v>28900</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="1" t="n">
         <v>3760</v>
       </c>
       <c r="C18" s="1"/>
@@ -3290,11 +1880,11 @@
       <c r="AV18" s="3"/>
       <c r="AW18" s="3"/>
     </row>
-    <row r="19" spans="1:49">
-      <c r="A19" s="1">
+    <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
         <v>32400</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="n">
         <v>4286</v>
       </c>
       <c r="C19" s="1"/>
@@ -3345,11 +1935,11 @@
       <c r="AV19" s="3"/>
       <c r="AW19" s="3"/>
     </row>
-    <row r="20" spans="1:49">
-      <c r="A20" s="1">
+    <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
         <v>36100</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="1" t="n">
         <v>4825</v>
       </c>
       <c r="C20" s="1"/>
@@ -3400,11 +1990,11 @@
       <c r="AV20" s="3"/>
       <c r="AW20" s="3"/>
     </row>
-    <row r="21" spans="1:49">
-      <c r="A21" s="1">
+    <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
         <v>40000</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="1" t="n">
         <v>4507</v>
       </c>
       <c r="C21" s="1"/>
@@ -3455,7 +2045,7 @@
       <c r="AV21" s="3"/>
       <c r="AW21" s="3"/>
     </row>
-    <row r="22" spans="1:49">
+    <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -3506,7 +2096,7 @@
       <c r="AV22" s="3"/>
       <c r="AW22" s="3"/>
     </row>
-    <row r="23" spans="1:49">
+    <row r="23" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3557,7 +2147,7 @@
       <c r="AV23" s="3"/>
       <c r="AW23" s="3"/>
     </row>
-    <row r="24" spans="1:49">
+    <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -3608,7 +2198,7 @@
       <c r="AV24" s="3"/>
       <c r="AW24" s="3"/>
     </row>
-    <row r="25" spans="1:49">
+    <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3659,7 +2249,7 @@
       <c r="AV25" s="3"/>
       <c r="AW25" s="3"/>
     </row>
-    <row r="26" spans="1:49">
+    <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3710,7 +2300,7 @@
       <c r="AV26" s="3"/>
       <c r="AW26" s="3"/>
     </row>
-    <row r="27" spans="1:49">
+    <row r="27" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3761,7 +2351,7 @@
       <c r="AV27" s="3"/>
       <c r="AW27" s="3"/>
     </row>
-    <row r="28" spans="1:49">
+    <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3812,7 +2402,7 @@
       <c r="AV28" s="3"/>
       <c r="AW28" s="3"/>
     </row>
-    <row r="29" spans="1:49">
+    <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3863,7 +2453,7 @@
       <c r="AV29" s="3"/>
       <c r="AW29" s="3"/>
     </row>
-    <row r="30" spans="1:49">
+    <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3914,7 +2504,7 @@
       <c r="AV30" s="3"/>
       <c r="AW30" s="3"/>
     </row>
-    <row r="31" spans="1:49">
+    <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3965,7 +2555,7 @@
       <c r="AV31" s="3"/>
       <c r="AW31" s="3"/>
     </row>
-    <row r="32" spans="1:49">
+    <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4016,7 +2606,7 @@
       <c r="AV32" s="3"/>
       <c r="AW32" s="3"/>
     </row>
-    <row r="33" spans="1:49">
+    <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -4067,7 +2657,7 @@
       <c r="AV33" s="3"/>
       <c r="AW33" s="3"/>
     </row>
-    <row r="34" spans="1:49">
+    <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -4118,7 +2708,7 @@
       <c r="AV34" s="3"/>
       <c r="AW34" s="3"/>
     </row>
-    <row r="35" spans="1:49">
+    <row r="35" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -4169,7 +2759,7 @@
       <c r="AV35" s="3"/>
       <c r="AW35" s="3"/>
     </row>
-    <row r="36" spans="1:49">
+    <row r="36" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -4220,7 +2810,7 @@
       <c r="AV36" s="3"/>
       <c r="AW36" s="3"/>
     </row>
-    <row r="37" spans="1:49">
+    <row r="37" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -4271,7 +2861,7 @@
       <c r="AV37" s="3"/>
       <c r="AW37" s="3"/>
     </row>
-    <row r="38" spans="1:49">
+    <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -4322,7 +2912,7 @@
       <c r="AV38" s="3"/>
       <c r="AW38" s="3"/>
     </row>
-    <row r="39" spans="1:49">
+    <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -4373,7 +2963,7 @@
       <c r="AV39" s="3"/>
       <c r="AW39" s="3"/>
     </row>
-    <row r="40" spans="1:49">
+    <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -4424,7 +3014,7 @@
       <c r="AV40" s="3"/>
       <c r="AW40" s="3"/>
     </row>
-    <row r="41" spans="1:49">
+    <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -4475,7 +3065,7 @@
       <c r="AV41" s="3"/>
       <c r="AW41" s="3"/>
     </row>
-    <row r="42" spans="1:49">
+    <row r="42" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -4526,7 +3116,7 @@
       <c r="AV42" s="3"/>
       <c r="AW42" s="3"/>
     </row>
-    <row r="43" spans="1:49">
+    <row r="43" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -4577,7 +3167,7 @@
       <c r="AV43" s="3"/>
       <c r="AW43" s="3"/>
     </row>
-    <row r="44" spans="1:49">
+    <row r="44" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -4628,7 +3218,7 @@
       <c r="AV44" s="3"/>
       <c r="AW44" s="3"/>
     </row>
-    <row r="45" spans="1:49">
+    <row r="45" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -4679,7 +3269,7 @@
       <c r="AV45" s="3"/>
       <c r="AW45" s="3"/>
     </row>
-    <row r="46" spans="1:49">
+    <row r="46" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -4731,8 +3321,13 @@
       <c r="AW46" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>